<commit_message>
Add MFR and some replace info
</commit_message>
<xml_diff>
--- a/PARTSLIST/Infinitas BOM.xlsx
+++ b/PARTSLIST/Infinitas BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF6167B-1553-4FCD-9F1E-1D1DE615818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9304A7B6-3698-4F38-BB4E-F831ADDAFAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="267">
   <si>
     <t>[Infinitas] Core rev 1.0.0 BOM</t>
   </si>
@@ -828,13 +828,22 @@
   </si>
   <si>
     <t>MFR</t>
+  </si>
+  <si>
+    <t>potentially replaceable</t>
+  </si>
+  <si>
+    <t>not potentially replaceable</t>
+  </si>
+  <si>
+    <t>Replaceable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -855,6 +864,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Courier New"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -930,7 +945,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -968,6 +983,9 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2132,9 +2150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -2145,20 +2163,21 @@
     <col min="4" max="4" width="31" style="1" customWidth="1"/>
     <col min="5" max="6" width="45.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="31" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.6" customHeight="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" ht="12" customHeight="1">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="12" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2180,8 +2199,11 @@
       <c r="G2" s="3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="24.6" customHeight="1">
+      <c r="H2" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="24.6" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2201,8 +2223,9 @@
         <v>8</v>
       </c>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="46.35" customHeight="1">
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="46.35" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -2224,8 +2247,11 @@
       <c r="G4" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="112.35" customHeight="1">
+      <c r="H4" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="112.35" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -2247,8 +2273,11 @@
       <c r="G5" s="6" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H5" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.35" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2270,8 +2299,11 @@
       <c r="G6" s="6" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H6" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="13.35" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -2293,8 +2325,11 @@
       <c r="G7" s="6" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H7" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.35" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
@@ -2316,8 +2351,11 @@
       <c r="G8" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="101.45" customHeight="1">
+      <c r="H8" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="101.45" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -2339,8 +2377,11 @@
       <c r="G9" s="6" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H9" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.35" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -2362,8 +2403,11 @@
       <c r="G10" s="6" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H10" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13.35" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -2385,8 +2429,11 @@
       <c r="G11" s="6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H11" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13.35" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
@@ -2408,8 +2455,11 @@
       <c r="G12" s="6" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H12" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="13.35" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -2428,11 +2478,14 @@
       <c r="F13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H13" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="13.35" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>54</v>
       </c>
@@ -2454,8 +2507,11 @@
       <c r="G14" s="6" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H14" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="13.35" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>59</v>
       </c>
@@ -2477,8 +2533,11 @@
       <c r="G15" s="6" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H15" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="13.35" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
@@ -2500,8 +2559,11 @@
       <c r="G16" s="6" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H16" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="13.35" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>69</v>
       </c>
@@ -2523,8 +2585,11 @@
       <c r="G17" s="6" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H17" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="13.35" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>72</v>
       </c>
@@ -2546,8 +2611,11 @@
       <c r="G18" s="6" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H18" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13.35" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>77</v>
       </c>
@@ -2569,8 +2637,11 @@
       <c r="G19" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H19" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="13.35" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
@@ -2592,8 +2663,11 @@
       <c r="G20" s="6" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H20" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13.35" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>87</v>
       </c>
@@ -2615,8 +2689,11 @@
       <c r="G21" s="6" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H21" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="13.35" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>92</v>
       </c>
@@ -2638,8 +2715,11 @@
       <c r="G22" s="6" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H22" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="13.35" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>97</v>
       </c>
@@ -2661,8 +2741,11 @@
       <c r="G23" s="6" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H23" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="13.35" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -2684,8 +2767,11 @@
       <c r="G24" s="6" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="24.4" customHeight="1">
+      <c r="H24" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="24.4" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>104</v>
       </c>
@@ -2707,8 +2793,11 @@
       <c r="G25" s="6" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H25" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13.35" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>109</v>
       </c>
@@ -2730,8 +2819,11 @@
       <c r="G26" s="6" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="68.45" customHeight="1">
+      <c r="H26" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="68.45" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>112</v>
       </c>
@@ -2753,8 +2845,11 @@
       <c r="G27" s="6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="46.35" customHeight="1">
+      <c r="H27" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="46.35" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>115</v>
       </c>
@@ -2776,8 +2871,11 @@
       <c r="G28" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="68.45" customHeight="1">
+      <c r="H28" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="68.45" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>118</v>
       </c>
@@ -2799,8 +2897,11 @@
       <c r="G29" s="6" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="46.35" customHeight="1">
+      <c r="H29" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="46.35" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>123</v>
       </c>
@@ -2822,8 +2923,11 @@
       <c r="G30" s="6" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H30" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="13.35" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>125</v>
       </c>
@@ -2845,8 +2949,11 @@
       <c r="G31" s="6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H31" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="13.35" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>128</v>
       </c>
@@ -2868,8 +2975,11 @@
       <c r="G32" s="6" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H32" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="13.35" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>131</v>
       </c>
@@ -2891,8 +3001,11 @@
       <c r="G33" s="6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H33" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="13.35" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>134</v>
       </c>
@@ -2914,8 +3027,11 @@
       <c r="G34" s="6" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H34" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="13.35" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>137</v>
       </c>
@@ -2937,8 +3053,11 @@
       <c r="G35" s="6" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H35" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="13.35" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>140</v>
       </c>
@@ -2960,8 +3079,11 @@
       <c r="G36" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H36" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="13.35" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>143</v>
       </c>
@@ -2983,8 +3105,11 @@
       <c r="G37" s="6" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H37" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="13.35" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>147</v>
       </c>
@@ -3003,11 +3128,14 @@
       <c r="F38" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="13" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H38" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="13.35" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>150</v>
       </c>
@@ -3029,8 +3157,11 @@
       <c r="G39" s="6" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H39" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="13.35" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>154</v>
       </c>
@@ -3052,8 +3183,11 @@
       <c r="G40" s="6" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H40" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="13.35" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>158</v>
       </c>
@@ -3075,8 +3209,11 @@
       <c r="G41" s="6" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H41" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="13.35" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>162</v>
       </c>
@@ -3098,8 +3235,11 @@
       <c r="G42" s="6" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H42" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="13.35" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>166</v>
       </c>
@@ -3121,8 +3261,11 @@
       <c r="G43" s="6">
         <v>61300411121</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H43" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="13.35" customHeight="1">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="8"/>
@@ -3130,8 +3273,9 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" ht="13.35" customHeight="1">
       <c r="A45" s="10" t="s">
         <v>170</v>
       </c>
@@ -3141,8 +3285,9 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="1:7" ht="24.4" customHeight="1">
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="1:8" ht="24.4" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>171</v>
       </c>
@@ -3164,8 +3309,11 @@
       <c r="G46" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="46.35" customHeight="1">
+      <c r="H46" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="46.35" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>172</v>
       </c>
@@ -3187,8 +3335,11 @@
       <c r="G47" s="6" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H47" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="13.35" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>173</v>
       </c>
@@ -3210,8 +3361,11 @@
       <c r="G48" s="6" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H48" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="13.35" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>176</v>
       </c>
@@ -3233,8 +3387,11 @@
       <c r="G49" s="6" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H49" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="13.35" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>180</v>
       </c>
@@ -3256,8 +3413,11 @@
       <c r="G50" s="6" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H50" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="13.35" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>184</v>
       </c>
@@ -3276,11 +3436,14 @@
       <c r="F51" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="G51" s="13" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H51" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="13.35" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>188</v>
       </c>
@@ -3302,8 +3465,11 @@
       <c r="G52" s="6" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H52" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="13.35" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>193</v>
       </c>
@@ -3325,8 +3491,11 @@
       <c r="G53" s="6">
         <v>61300211121</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H53" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="13.35" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>197</v>
       </c>
@@ -3348,8 +3517,11 @@
       <c r="G54" s="6" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H54" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="13.35" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>202</v>
       </c>
@@ -3371,8 +3543,11 @@
       <c r="G55" s="6" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="24.4" customHeight="1">
+      <c r="H55" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="24.4" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>203</v>
       </c>
@@ -3394,8 +3569,11 @@
       <c r="G56" s="6" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H56" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="13.35" customHeight="1">
       <c r="A57" s="6" t="s">
         <v>204</v>
       </c>
@@ -3417,8 +3595,11 @@
       <c r="G57" s="6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H57" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="13.35" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>205</v>
       </c>
@@ -3440,8 +3621,11 @@
       <c r="G58" s="6" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="24.4" customHeight="1">
+      <c r="H58" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="24.4" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>208</v>
       </c>
@@ -3461,8 +3645,9 @@
         <v>8</v>
       </c>
       <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="1:7" ht="24.4" customHeight="1">
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8" ht="24.4" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>210</v>
       </c>
@@ -3484,8 +3669,11 @@
       <c r="G60" s="6" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="13.35" customHeight="1">
+      <c r="H60" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="13.35" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>213</v>
       </c>
@@ -3506,6 +3694,9 @@
       </c>
       <c r="G61" s="6" t="s">
         <v>257</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>